<commit_message>
Moved recovery rate and premium frequency of cds to data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasiraj/Library/CloudStorage/OneDrive-UniversityofGlasgow/Industry Project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasiraj/Library/CloudStorage/OneDrive-UniversityofGlasgow/Industry Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6724BF27-5DC3-B141-9FD8-AB05B8A9CF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E101F7-F970-2043-8369-5AEA28F285B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="1140" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
+    <workbookView xWindow="10760" yWindow="1140" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
   </bookViews>
   <sheets>
     <sheet name="interest_rate_term_structure" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>rate</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>years</t>
+  </si>
+  <si>
+    <t>recovery_rate</t>
+  </si>
+  <si>
+    <t>premium_frequency</t>
   </si>
 </sst>
 </file>
@@ -1333,7 +1339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF84E3C-6123-564C-ACEF-26D67C5C8B64}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -1535,15 +1541,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE280868-0661-6A4B-9B03-0147465E5A5C}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1556,8 +1562,14 @@
       <c r="D1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.35420099999999999</v>
       </c>
@@ -1569,6 +1581,12 @@
       </c>
       <c r="D2">
         <v>1.8100000000000002E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.4</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inital CLV calculation for 81 tranches
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasiraj/Library/CloudStorage/OneDrive-UniversityofGlasgow/Industry Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E101F7-F970-2043-8369-5AEA28F285B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761125F9-5608-1D48-8EFC-8EA192E8A0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="1140" windowWidth="27640" windowHeight="16940" activeTab="3" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
+    <workbookView xWindow="11700" yWindow="1320" windowWidth="26700" windowHeight="16940" activeTab="4" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
   </bookViews>
   <sheets>
     <sheet name="interest_rate_term_structure" sheetId="1" r:id="rId1"/>
-    <sheet name="credit_risk_term_structure" sheetId="2" r:id="rId2"/>
-    <sheet name="interest_rate_parameters" sheetId="3" r:id="rId3"/>
-    <sheet name="credit_risk_parameters" sheetId="4" r:id="rId4"/>
+    <sheet name="test" sheetId="5" r:id="rId2"/>
+    <sheet name="credit_risk_term_structure" sheetId="2" r:id="rId3"/>
+    <sheet name="interest_rate_parameters" sheetId="3" r:id="rId4"/>
+    <sheet name="credit_risk_parameters" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>rate</t>
   </si>
@@ -76,15 +77,19 @@
   <si>
     <t>premium_frequency</t>
   </si>
+  <si>
+    <t>rate %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00##_);[Red]\(#,##0.00##\)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -97,6 +102,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,11 +131,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="blp_amount" xfId="1" xr:uid="{219DA6DC-62C8-8041-9DCD-56D79194C870}"/>
@@ -440,16 +455,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B238863E-1E4E-CE48-8256-D2C0605750DF}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66:B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -471,14 +486,14 @@
         <v>7</v>
       </c>
       <c r="B2" s="1">
-        <v>5.2441946705752089</v>
+        <v>5.214953800441835</v>
       </c>
       <c r="C2">
-        <f t="shared" ref="C2:C55" si="0">B2*0.01</f>
-        <v>5.2441946705752092E-2</v>
+        <f t="shared" ref="C2:C65" si="0">B2*0.01</f>
+        <v>5.214953800441835E-2</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:D55" si="1">A2/12</f>
+        <f t="shared" ref="D2:D65" si="1">A2/12</f>
         <v>0.58333333333333337</v>
       </c>
     </row>
@@ -487,11 +502,11 @@
         <v>8</v>
       </c>
       <c r="B3" s="1">
-        <v>5.2732754749610073</v>
+        <v>5.2499208623398141</v>
       </c>
       <c r="C3">
         <f t="shared" si="0"/>
-        <v>5.2732754749610075E-2</v>
+        <v>5.2499208623398144E-2</v>
       </c>
       <c r="D3">
         <f t="shared" si="1"/>
@@ -503,11 +518,11 @@
         <v>9</v>
       </c>
       <c r="B4" s="1">
-        <v>5.2975380606702176</v>
+        <v>5.2793225272611943</v>
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>5.2975380606702177E-2</v>
+        <v>5.2793225272611946E-2</v>
       </c>
       <c r="D4">
         <f t="shared" si="1"/>
@@ -519,11 +534,11 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>5.3173191828803406</v>
+        <v>5.303614331513959</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>5.3173191828803409E-2</v>
+        <v>5.3036143315139589E-2</v>
       </c>
       <c r="D5">
         <f t="shared" si="1"/>
@@ -535,11 +550,11 @@
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>5.3330643663968456</v>
+        <v>5.3233783667883481</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>5.3330643663968454E-2</v>
+        <v>5.3233783667883484E-2</v>
       </c>
       <c r="D6">
         <f t="shared" si="1"/>
@@ -551,11 +566,11 @@
         <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>5.3451955542696608</v>
+        <v>5.3391442378202791</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>5.3451955542696605E-2</v>
+        <v>5.3391442378202793E-2</v>
       </c>
       <c r="D7">
         <f t="shared" si="1"/>
@@ -567,11 +582,11 @@
         <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>5.3540842738722958</v>
+        <v>5.3513643142639609</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>5.3540842738722956E-2</v>
+        <v>5.3513643142639608E-2</v>
       </c>
       <c r="D8">
         <f t="shared" si="1"/>
@@ -583,11 +598,11 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>5.3600687944653789</v>
+        <v>5.3604405318685737</v>
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>5.3600687944653787E-2</v>
+        <v>5.3604405318685738E-2</v>
       </c>
       <c r="D9">
         <f t="shared" si="1"/>
@@ -599,11 +614,11 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>5.3634645514365058</v>
+        <v>5.3667400838309574</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>5.3634645514365059E-2</v>
+        <v>5.3667400838309572E-2</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
@@ -615,11 +630,11 @@
         <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>5.3645567714425626</v>
+        <v>5.3705867245305461</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>5.3645567714425628E-2</v>
+        <v>5.3705867245305461E-2</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
@@ -631,11 +646,11 @@
         <v>17</v>
       </c>
       <c r="B12" s="1">
-        <v>5.363586512141385</v>
+        <v>5.372246886885665</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>5.3635865121413849E-2</v>
+        <v>5.3722468868856649E-2</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
@@ -647,11 +662,11 @@
         <v>18</v>
       </c>
       <c r="B13" s="1">
-        <v>5.3607591906408318</v>
+        <v>5.3719419322115476</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>5.360759190640832E-2</v>
+        <v>5.3719419322115478E-2</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
@@ -663,11 +678,11 @@
         <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>5.356253957873772</v>
+        <v>5.3698600095955884</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>5.3562539578737724E-2</v>
+        <v>5.3698600095955888E-2</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
@@ -679,11 +694,11 @@
         <v>20</v>
       </c>
       <c r="B15" s="1">
-        <v>5.3502298166241795</v>
+        <v>5.3661639878456731</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>5.3502298166241795E-2</v>
+        <v>5.3661639878456735E-2</v>
       </c>
       <c r="D15">
         <f t="shared" si="1"/>
@@ -695,11 +710,11 @@
         <v>21</v>
       </c>
       <c r="B16" s="1">
-        <v>5.3428262470717707</v>
+        <v>5.360994689455171</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>5.3428262470717705E-2</v>
+        <v>5.3609946894551709E-2</v>
       </c>
       <c r="D16">
         <f t="shared" si="1"/>
@@ -711,11 +726,11 @@
         <v>22</v>
       </c>
       <c r="B17" s="1">
-        <v>5.3341658514795496</v>
+        <v>5.3544757952510116</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>5.3341658514795498E-2</v>
+        <v>5.3544757952510118E-2</v>
       </c>
       <c r="D17">
         <f t="shared" si="1"/>
@@ -727,11 +742,11 @@
         <v>23</v>
       </c>
       <c r="B18" s="1">
-        <v>5.3243602772905465</v>
+        <v>5.3467197800329371</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>5.3243602772905463E-2</v>
+        <v>5.3467197800329373E-2</v>
       </c>
       <c r="D18">
         <f t="shared" si="1"/>
@@ -743,11 +758,11 @@
         <v>24</v>
       </c>
       <c r="B19" s="1">
-        <v>5.3135128182934492</v>
+        <v>5.3378305120534693</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>5.3135128182934491E-2</v>
+        <v>5.3378305120534694E-2</v>
       </c>
       <c r="D19">
         <f t="shared" si="1"/>
@@ -759,11 +774,11 @@
         <v>25</v>
       </c>
       <c r="B20" s="1">
-        <v>5.3017202008618485</v>
+        <v>5.3279053775003788</v>
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>5.3017202008618487E-2</v>
+        <v>5.327905377500379E-2</v>
       </c>
       <c r="D20">
         <f t="shared" si="1"/>
@@ -775,11 +790,11 @@
         <v>26</v>
       </c>
       <c r="B21" s="1">
-        <v>5.2890740228749653</v>
+        <v>5.3170370591848579</v>
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>5.2890740228749657E-2</v>
+        <v>5.3170370591848579E-2</v>
       </c>
       <c r="D21">
         <f t="shared" si="1"/>
@@ -791,11 +806,11 @@
         <v>27</v>
       </c>
       <c r="B22" s="1">
-        <v>5.2756617315409526</v>
+        <v>5.3053144821873568</v>
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>5.2756617315409531E-2</v>
+        <v>5.3053144821873566E-2</v>
       </c>
       <c r="D22">
         <f t="shared" si="1"/>
@@ -807,11 +822,11 @@
         <v>28</v>
       </c>
       <c r="B23" s="1">
-        <v>5.2615673728105126</v>
+        <v>5.2928235545948192</v>
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>5.2615673728105126E-2</v>
+        <v>5.2928235545948193E-2</v>
       </c>
       <c r="D23">
         <f t="shared" si="1"/>
@@ -823,11 +838,11 @@
         <v>29</v>
       </c>
       <c r="B24" s="1">
-        <v>5.2468716018740116</v>
+        <v>5.2796470546624041</v>
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>5.2468716018740119E-2</v>
+        <v>5.2796470546624043E-2</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
@@ -839,11 +854,11 @@
         <v>30</v>
       </c>
       <c r="B25" s="1">
-        <v>5.2316497777847175</v>
+        <v>5.2658625613141634</v>
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>5.2316497777847179E-2</v>
+        <v>5.2658625613141635E-2</v>
       </c>
       <c r="D25">
         <f t="shared" si="1"/>
@@ -855,11 +870,11 @@
         <v>31</v>
       </c>
       <c r="B26" s="1">
-        <v>5.2159717080883201</v>
+        <v>5.2515422847152706</v>
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>5.2159717080883204E-2</v>
+        <v>5.2515422847152708E-2</v>
       </c>
       <c r="D26">
         <f t="shared" si="1"/>
@@ -871,11 +886,11 @@
         <v>32</v>
       </c>
       <c r="B27" s="1">
-        <v>5.1999023276689584</v>
+        <v>5.2367536805783317</v>
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>5.1999023276689586E-2</v>
+        <v>5.2367536805783321E-2</v>
       </c>
       <c r="D27">
         <f t="shared" si="1"/>
@@ -887,11 +902,11 @@
         <v>33</v>
       </c>
       <c r="B28" s="1">
-        <v>5.1835010185853871</v>
+        <v>5.2215586501961591</v>
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>5.1835010185853875E-2</v>
+        <v>5.2215586501961592E-2</v>
       </c>
       <c r="D28">
         <f t="shared" si="1"/>
@@ -903,11 +918,11 @@
         <v>34</v>
       </c>
       <c r="B29" s="1">
-        <v>5.1668212267541094</v>
+        <v>5.2060132430023609</v>
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>5.1668212267541092E-2</v>
+        <v>5.2060132430023609E-2</v>
       </c>
       <c r="D29">
         <f t="shared" si="1"/>
@@ -919,11 +934,11 @@
         <v>35</v>
       </c>
       <c r="B30" s="1">
-        <v>5.1499112220841576</v>
+        <v>5.1901684260631962</v>
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>5.1499112220841581E-2</v>
+        <v>5.1901684260631964E-2</v>
       </c>
       <c r="D30">
         <f t="shared" si="1"/>
@@ -935,11 +950,11 @@
         <v>36</v>
       </c>
       <c r="B31" s="1">
-        <v>5.1328148173670263</v>
+        <v>5.1740707899619247</v>
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>5.1328148173670263E-2</v>
+        <v>5.1740707899619251E-2</v>
       </c>
       <c r="D31">
         <f t="shared" si="1"/>
@@ -951,11 +966,11 @@
         <v>37</v>
       </c>
       <c r="B32" s="1">
-        <v>5.1155719703204054</v>
+        <v>5.1577631394305463</v>
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>5.1155719703204053E-2</v>
+        <v>5.1577631394305462E-2</v>
       </c>
       <c r="D32">
         <f t="shared" si="1"/>
@@ -967,11 +982,11 @@
         <v>38</v>
       </c>
       <c r="B33" s="1">
-        <v>5.098219244852304</v>
+        <v>5.1412849082394345</v>
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>5.0982192448523041E-2</v>
+        <v>5.1412849082394345E-2</v>
       </c>
       <c r="D33">
         <f t="shared" si="1"/>
@@ -983,11 +998,11 @@
         <v>39</v>
       </c>
       <c r="B34" s="1">
-        <v>5.0807900640114676</v>
+        <v>5.1246723096298199</v>
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>5.080790064011468E-2</v>
+        <v>5.12467230962982E-2</v>
       </c>
       <c r="D34">
         <f t="shared" si="1"/>
@@ -999,11 +1014,11 @@
         <v>40</v>
       </c>
       <c r="B35" s="1">
-        <v>5.0633150246099543</v>
+        <v>5.1079586349227473</v>
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>5.0633150246099545E-2</v>
+        <v>5.1079586349227477E-2</v>
       </c>
       <c r="D35">
         <f t="shared" si="1"/>
@@ -1015,11 +1030,11 @@
         <v>41</v>
       </c>
       <c r="B36" s="1">
-        <v>5.0458222277927272</v>
+        <v>5.0911746019868076</v>
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>5.0458222277927275E-2</v>
+        <v>5.091174601986808E-2</v>
       </c>
       <c r="D36">
         <f t="shared" si="1"/>
@@ -1031,11 +1046,11 @@
         <v>42</v>
       </c>
       <c r="B37" s="1">
-        <v>5.028337524601433</v>
+        <v>5.0743486398930564</v>
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>5.0283375246014332E-2</v>
+        <v>5.0743486398930567E-2</v>
       </c>
       <c r="D37">
         <f t="shared" si="1"/>
@@ -1047,11 +1062,11 @@
         <v>43</v>
       </c>
       <c r="B38" s="1">
-        <v>5.010884754274433</v>
+        <v>5.057507146564344</v>
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>5.0108847542744334E-2</v>
+        <v>5.057507146564344E-2</v>
       </c>
       <c r="D38">
         <f t="shared" si="1"/>
@@ -1063,11 +1078,11 @@
         <v>44</v>
       </c>
       <c r="B39" s="1">
-        <v>4.9934859628081663</v>
+        <v>5.0406746987379067</v>
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>4.9934859628081661E-2</v>
+        <v>5.040674698737907E-2</v>
       </c>
       <c r="D39">
         <f t="shared" si="1"/>
@@ -1079,11 +1094,11 @@
         <v>45</v>
       </c>
       <c r="B40" s="1">
-        <v>4.9761615249252555</v>
+        <v>5.0238741126131119</v>
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>4.9761615249252558E-2</v>
+        <v>5.0238741126131123E-2</v>
       </c>
       <c r="D40">
         <f t="shared" si="1"/>
@@ -1095,11 +1110,11 @@
         <v>46</v>
       </c>
       <c r="B41" s="1">
-        <v>4.9589302644027375</v>
+        <v>5.0071265377841732</v>
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>4.9589302644027375E-2</v>
+        <v>5.0071265377841734E-2</v>
       </c>
       <c r="D41">
         <f t="shared" si="1"/>
@@ -1111,11 +1126,11 @@
         <v>47</v>
       </c>
       <c r="B42" s="1">
-        <v>4.9418096149754289</v>
+        <v>4.9904516292762668</v>
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>4.9418096149754287E-2</v>
+        <v>4.9904516292762671E-2</v>
       </c>
       <c r="D42">
         <f t="shared" si="1"/>
@@ -1127,11 +1142,11 @@
         <v>48</v>
       </c>
       <c r="B43" s="1">
-        <v>4.924815765131993</v>
+        <v>4.9738677032298018</v>
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>4.9248157651319929E-2</v>
+        <v>4.973867703229802E-2</v>
       </c>
       <c r="D43">
         <f t="shared" si="1"/>
@@ -1143,11 +1158,11 @@
         <v>49</v>
       </c>
       <c r="B44" s="1">
-        <v>4.9079637848299216</v>
+        <v>4.9573918728458848</v>
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>4.9079637848299218E-2</v>
+        <v>4.957391872845885E-2</v>
       </c>
       <c r="D44">
         <f t="shared" si="1"/>
@@ -1159,11 +1174,11 @@
         <v>50</v>
       </c>
       <c r="B45" s="1">
-        <v>4.891267677066331</v>
+        <v>4.9410400965757368</v>
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>4.8912676770663313E-2</v>
+        <v>4.941040096575737E-2</v>
       </c>
       <c r="D45">
         <f t="shared" si="1"/>
@@ -1175,11 +1190,11 @@
         <v>51</v>
       </c>
       <c r="B46" s="1">
-        <v>4.8747402422024857</v>
+        <v>4.9248270457938244</v>
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>4.8747402422024855E-2</v>
+        <v>4.9248270457938247E-2</v>
       </c>
       <c r="D46">
         <f t="shared" si="1"/>
@@ -1191,11 +1206,11 @@
         <v>52</v>
       </c>
       <c r="B47" s="1">
-        <v>4.8583930902002121</v>
+        <v>4.9087661374626981</v>
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>4.8583930902002123E-2</v>
+        <v>4.908766137462698E-2</v>
       </c>
       <c r="D47">
         <f t="shared" si="1"/>
@@ -1207,11 +1222,11 @@
         <v>53</v>
       </c>
       <c r="B48" s="1">
-        <v>4.8422367504346937</v>
+        <v>4.8928696508640783</v>
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>4.842236750434694E-2</v>
+        <v>4.8928696508640783E-2</v>
       </c>
       <c r="D48">
         <f t="shared" si="1"/>
@@ -1223,11 +1238,11 @@
         <v>54</v>
       </c>
       <c r="B49" s="1">
-        <v>4.8262807731638082</v>
+        <v>4.8771488346177065</v>
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>4.8262807731638081E-2</v>
+        <v>4.8771488346177068E-2</v>
       </c>
       <c r="D49">
         <f t="shared" si="1"/>
@@ -1239,11 +1254,11 @@
         <v>55</v>
       </c>
       <c r="B50" s="1">
-        <v>4.8105338437143184</v>
+        <v>4.8616140245526651</v>
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>4.8105338437143187E-2</v>
+        <v>4.861614024552665E-2</v>
       </c>
       <c r="D50">
         <f t="shared" si="1"/>
@@ -1255,11 +1270,11 @@
         <v>56</v>
       </c>
       <c r="B51" s="1">
-        <v>4.7950038944916082</v>
+        <v>4.8462747495320908</v>
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>4.7950038944916083E-2</v>
+        <v>4.846274749532091E-2</v>
       </c>
       <c r="D51">
         <f t="shared" si="1"/>
@@ -1271,11 +1286,11 @@
         <v>57</v>
       </c>
       <c r="B52" s="1">
-        <v>4.7796981720229974</v>
+        <v>4.8311397649751058</v>
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>4.7796981720229975E-2</v>
+        <v>4.8311397649751057E-2</v>
       </c>
       <c r="D52">
         <f t="shared" si="1"/>
@@ -1287,11 +1302,11 @@
         <v>58</v>
       </c>
       <c r="B53" s="1">
-        <v>4.7646232924660987</v>
+        <v>4.8162170870880301</v>
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>4.764623292466099E-2</v>
+        <v>4.8162170870880303E-2</v>
       </c>
       <c r="D53">
         <f t="shared" si="1"/>
@@ -1303,11 +1318,11 @@
         <v>59</v>
       </c>
       <c r="B54" s="1">
-        <v>4.7497852947337913</v>
+        <v>4.80151405333587</v>
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>4.7497852947337917E-2</v>
+        <v>4.8015140533358702E-2</v>
       </c>
       <c r="D54">
         <f t="shared" si="1"/>
@@ -1319,15 +1334,175 @@
         <v>60</v>
       </c>
       <c r="B55" s="1">
-        <v>4.7351896885979494</v>
+        <v>4.7870373790040857</v>
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>4.7351896885979496E-2</v>
+        <v>4.787037379004086E-2</v>
       </c>
       <c r="D55">
         <f t="shared" si="1"/>
         <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>66</v>
+      </c>
+      <c r="B56" s="1">
+        <v>4.7052400315038305</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>4.7052400315038309E-2</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>72</v>
+      </c>
+      <c r="B57" s="1">
+        <v>4.6327313095291256</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>4.6327313095291256E-2</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>78</v>
+      </c>
+      <c r="B58" s="1">
+        <v>4.5699854728424292</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>4.5699854728424291E-2</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>84</v>
+      </c>
+      <c r="B59" s="1">
+        <v>4.5171153350614226</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>4.5171153350614224E-2</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>90</v>
+      </c>
+      <c r="B60" s="1">
+        <v>4.4739310785747044</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>4.4739310785747048E-2</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>96</v>
+      </c>
+      <c r="B61" s="1">
+        <v>4.4400069766965471</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>4.4400069766965471E-2</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>102</v>
+      </c>
+      <c r="B62" s="1">
+        <v>4.4147225511382011</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>4.4147225511382011E-2</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>108</v>
+      </c>
+      <c r="B63" s="1">
+        <v>4.3973084873371873</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>4.397308487337187E-2</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>114</v>
+      </c>
+      <c r="B64" s="1">
+        <v>4.3868966918137655</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>4.3868966918137658E-2</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>120</v>
+      </c>
+      <c r="B65" s="1">
+        <v>4.3825526508538601</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>4.3825526508538604E-2</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1336,6 +1511,992 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D5C0D8-ECF6-5048-8A3F-F142108CDAFC}">
+  <dimension ref="A1:C81"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>0.75167073638756288</v>
+      </c>
+      <c r="B2">
+        <f>A2/100</f>
+        <v>7.5167073638756285E-3</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0.75145078980616009</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B66" si="0">A3/100</f>
+        <v>7.5145078980616009E-3</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.76512965913807485</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>7.6512965913807483E-3</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0.79993264917340767</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>7.9993264917340764E-3</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>0.84722222812211745</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>8.4722222812211746E-3</v>
+      </c>
+      <c r="C6" s="4">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>0.90053184539969944</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>9.0053184539969945E-3</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>0.95606556439557744</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>9.5606556439557736E-3</v>
+      </c>
+      <c r="C8" s="4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1.0116682594176742</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>1.0116682594176743E-2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1.0661472831649033</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>1.0661472831649033E-2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1.1189161304229813</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>1.1189161304229813E-2</v>
+      </c>
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>1.1697595209056226</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>1.1697595209056227E-2</v>
+      </c>
+      <c r="C12" s="5">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>1.2186913841294837</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>1.2186913841294838E-2</v>
+      </c>
+      <c r="C13" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1.2658400685316418</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>1.2658400685316418E-2</v>
+      </c>
+      <c r="C14" s="5">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>1.3113708849466152</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1.3113708849466152E-2</v>
+      </c>
+      <c r="C15" s="5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>1.3554354856683479</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>1.3554354856683479E-2</v>
+      </c>
+      <c r="C16" s="5">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>1.398147173164731</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>1.3981471731647311E-2</v>
+      </c>
+      <c r="C17" s="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>1.439579062599309</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>1.4395790625993089E-2</v>
+      </c>
+      <c r="C18" s="5">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>1.4797662889469168</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>1.4797662889469168E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>1.5187113555377778</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>1.5187113555377779E-2</v>
+      </c>
+      <c r="C20" s="5">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>1.5563891771978171</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1.556389177197817E-2</v>
+      </c>
+      <c r="C21" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>1.5927557618344945</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1.5927557618344947E-2</v>
+      </c>
+      <c r="C22" s="5">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>1.627752949036102</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1.6277529490361022E-2</v>
+      </c>
+      <c r="C23" s="5">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>1.6613236262807265</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>1.6613236262807266E-2</v>
+      </c>
+      <c r="C24" s="5">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>1.6934152853734599</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>1.6934152853734598E-2</v>
+      </c>
+      <c r="C25" s="5">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>1.7239792810951982</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>1.7239792810951983E-2</v>
+      </c>
+      <c r="C26" s="5">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>1.7529745565451949</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>1.7529745565451949E-2</v>
+      </c>
+      <c r="C27" s="5">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>1.7803741636598349</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1.7803741636598348E-2</v>
+      </c>
+      <c r="C28" s="5">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>1.8061642647584863</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1.8061642647584863E-2</v>
+      </c>
+      <c r="C29" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>1.8303428713728076</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>1.8303428713728077E-2</v>
+      </c>
+      <c r="C30" s="5">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>1.8529196109680839</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>1.8529196109680839E-2</v>
+      </c>
+      <c r="C31" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>1.8739141735445437</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>1.8739141735445438E-2</v>
+      </c>
+      <c r="C32" s="5">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>1.8933547400396706</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>1.8933547400396707E-2</v>
+      </c>
+      <c r="C33" s="5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>1.9112767162113791</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>1.911276716211379E-2</v>
+      </c>
+      <c r="C34" s="5">
+        <v>16.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>1.9277217875947581</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>1.9277217875947581E-2</v>
+      </c>
+      <c r="C35" s="5">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>1.9427370915825841</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>1.9427370915825842E-2</v>
+      </c>
+      <c r="C36" s="5">
+        <v>17.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>1.9563739207142961</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>1.9563739207142959E-2</v>
+      </c>
+      <c r="C37" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>1.968684050984419</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>1.9686840509844192E-2</v>
+      </c>
+      <c r="C38" s="5">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>1.9797178349578859</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1.9797178349578858E-2</v>
+      </c>
+      <c r="C39" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>1.9895243051730016</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>1.9895243051730016E-2</v>
+      </c>
+      <c r="C40" s="5">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>1.9981513391447703</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>1.9981513391447703E-2</v>
+      </c>
+      <c r="C41" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>2.0056457476480816</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>2.0056457476480816E-2</v>
+      </c>
+      <c r="C42" s="5">
+        <v>20.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>2.0120519901173344</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>2.0120519901173344E-2</v>
+      </c>
+      <c r="C43" s="5">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>2.0174101476459754</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>2.0174101476459753E-2</v>
+      </c>
+      <c r="C44" s="5">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>2.0217573495520753</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>2.0217573495520752E-2</v>
+      </c>
+      <c r="C45" s="5">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>2.0251289801612935</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>2.0251289801612934E-2</v>
+      </c>
+      <c r="C46" s="5">
+        <v>22.5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>2.0275595983600017</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>2.0275595983600018E-2</v>
+      </c>
+      <c r="C47" s="5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>2.0290842880828004</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>2.0290842880828004E-2</v>
+      </c>
+      <c r="C48" s="5">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>2.0297388467590118</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>2.0297388467590119E-2</v>
+      </c>
+      <c r="C49" s="5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>2.0295597395088429</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>2.0295597395088429E-2</v>
+      </c>
+      <c r="C50" s="5">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>2.0285847752476664</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>2.0285847752476664E-2</v>
+      </c>
+      <c r="C51" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>2.0268543512710573</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>2.0268543512710572E-2</v>
+      </c>
+      <c r="C52" s="5">
+        <v>25.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>2.0244116538022507</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>2.0244116538022508E-2</v>
+      </c>
+      <c r="C53" s="5">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>2.0213029785141878</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>2.0213029785141879E-2</v>
+      </c>
+      <c r="C54" s="5">
+        <v>26.5</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>2.0175774747600119</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>2.0175774747600118E-2</v>
+      </c>
+      <c r="C55" s="5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>2.0132863100478877</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>2.0132863100478876E-2</v>
+      </c>
+      <c r="C56" s="5">
+        <v>27.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>2.0084822799182072</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>2.008482279918207E-2</v>
+      </c>
+      <c r="C57" s="5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>2.0032196414153747</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>2.0032196414153748E-2</v>
+      </c>
+      <c r="C58" s="5">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>1.9975534145387082</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>1.997553414538708E-2</v>
+      </c>
+      <c r="C59" s="5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>1.99153800135746</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>1.99153800135746E-2</v>
+      </c>
+      <c r="C60" s="5">
+        <v>29.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>1.9852261944736576</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>1.9852261944736577E-2</v>
+      </c>
+      <c r="C61" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>1.9786690136576981</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>1.9786690136576982E-2</v>
+      </c>
+      <c r="C62" s="5">
+        <v>30.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>1.9719157633862983</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>1.9719157633862984E-2</v>
+      </c>
+      <c r="C63" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>1.9650138865784179</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>1.9650138865784178E-2</v>
+      </c>
+      <c r="C64" s="5">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>1.9580086340046001</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>1.9580086340046002E-2</v>
+      </c>
+      <c r="C65" s="5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>1.9509425199502524</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>1.9509425199502523E-2</v>
+      </c>
+      <c r="C66" s="5">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>1.9438553879025715</v>
+      </c>
+      <c r="B67">
+        <f t="shared" ref="B67:B81" si="1">A67/100</f>
+        <v>1.9438553879025714E-2</v>
+      </c>
+      <c r="C67" s="5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>1.9367846094794383</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="1"/>
+        <v>1.9367846094794382E-2</v>
+      </c>
+      <c r="C68" s="5">
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>1.9297652641804675</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="1"/>
+        <v>1.9297652641804674E-2</v>
+      </c>
+      <c r="C69" s="5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>1.9228301085760584</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="1"/>
+        <v>1.9228301085760582E-2</v>
+      </c>
+      <c r="C70" s="5">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>1.9160090894949462</v>
+      </c>
+      <c r="B71">
+        <f t="shared" si="1"/>
+        <v>1.9160090894949463E-2</v>
+      </c>
+      <c r="C71" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>1.9093293059487111</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="1"/>
+        <v>1.909329305948711E-2</v>
+      </c>
+      <c r="C72" s="5">
+        <v>35.5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>1.9028152029879071</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="1"/>
+        <v>1.9028152029879071E-2</v>
+      </c>
+      <c r="C73" s="5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="1">
+        <v>1.8964887534802075</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="1"/>
+        <v>1.8964887534802074E-2</v>
+      </c>
+      <c r="C74" s="5">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>1.890369625149797</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="1"/>
+        <v>1.8903696251497969E-2</v>
+      </c>
+      <c r="C75" s="5">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>1.8844753323633274</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="1"/>
+        <v>1.8844753323633275E-2</v>
+      </c>
+      <c r="C76" s="5">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="1">
+        <v>1.8788213219358558</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="1"/>
+        <v>1.8788213219358557E-2</v>
+      </c>
+      <c r="C77" s="5">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>1.8734210007897918</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="1"/>
+        <v>1.873421000789792E-2</v>
+      </c>
+      <c r="C78" s="5">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>1.8682858444945127</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="1"/>
+        <v>1.8682858444945126E-2</v>
+      </c>
+      <c r="C79" s="5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>1.8634254502936896</v>
+      </c>
+      <c r="B80">
+        <f t="shared" si="1"/>
+        <v>1.8634254502936896E-2</v>
+      </c>
+      <c r="C80" s="5">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>1.8588474188546644</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>1.8588474188546644E-2</v>
+      </c>
+      <c r="C81" s="5">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF84E3C-6123-564C-ACEF-26D67C5C8B64}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1496,17 +2657,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676432AF-0F53-454C-A2CE-3A93B5AF25D7}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1520,18 +2681,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0.52890499999999996</v>
       </c>
       <c r="B2">
-        <v>3.1990400000000002E-2</v>
+        <v>2.6499999999999999E-2</v>
       </c>
       <c r="C2">
         <v>0.13003500000000001</v>
       </c>
       <c r="D2" s="3">
         <v>8.3234900000000005E-5</v>
+      </c>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>3.1990400000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>0.13003500000000001</v>
       </c>
     </row>
   </sheetData>
@@ -1539,15 +2709,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE280868-0661-6A4B-9B03-0147465E5A5C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1580,7 +2753,7 @@
         <v>2.38186E-3</v>
       </c>
       <c r="D2">
-        <v>1.8100000000000002E-2</v>
+        <v>1.81E-3</v>
       </c>
       <c r="E2">
         <v>0.4</v>

</xml_diff>

<commit_message>
Add yield curves and curves for cds hazard rate
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,19 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasiraj/Library/CloudStorage/OneDrive-UniversityofGlasgow/Industry Project/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2764405r_student_gla_ac_uk/Documents/Industry Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761125F9-5608-1D48-8EFC-8EA192E8A0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8EF8A760-6F87-3F47-B0D2-BB4510910C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB22C586-A602-C341-9088-DF4A6ADD63F8}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="1320" windowWidth="26700" windowHeight="16940" activeTab="4" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
+    <workbookView xWindow="11700" yWindow="1700" windowWidth="26700" windowHeight="16940" activeTab="1" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
   </bookViews>
   <sheets>
     <sheet name="interest_rate_term_structure" sheetId="1" r:id="rId1"/>
-    <sheet name="test" sheetId="5" r:id="rId2"/>
-    <sheet name="credit_risk_term_structure" sheetId="2" r:id="rId3"/>
-    <sheet name="interest_rate_parameters" sheetId="3" r:id="rId4"/>
-    <sheet name="credit_risk_parameters" sheetId="4" r:id="rId5"/>
+    <sheet name="credit_risk_term_structure" sheetId="2" r:id="rId2"/>
+    <sheet name="interest_rate_parameters" sheetId="3" r:id="rId3"/>
+    <sheet name="credit_risk_parameters" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
   <si>
     <t>rate</t>
   </si>
@@ -77,19 +76,15 @@
   <si>
     <t>premium_frequency</t>
   </si>
-  <si>
-    <t>rate %</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00##_);[Red]\(#,##0.00##\)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,12 +97,6 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -131,15 +120,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="blp_amount" xfId="1" xr:uid="{219DA6DC-62C8-8041-9DCD-56D79194C870}"/>
@@ -457,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B238863E-1E4E-CE48-8256-D2C0605750DF}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B125"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="B2" sqref="A1:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,985 +1496,168 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D5C0D8-ECF6-5048-8A3F-F142108CDAFC}">
-  <dimension ref="A1:C81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF84E3C-6123-564C-ACEF-26D67C5C8B64}">
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <f>A2/12</f>
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <f>D2*0.0001</f>
+        <v>8.1129268646200001E-3</v>
+      </c>
+      <c r="D2" s="2">
+        <v>81.129268646200003</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0.75167073638756288</v>
-      </c>
-      <c r="B2">
-        <f>A2/100</f>
-        <v>7.5167073638756285E-3</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0.75145078980616009</v>
-      </c>
       <c r="B3">
-        <f t="shared" ref="B3:B66" si="0">A3/100</f>
-        <v>7.5145078980616009E-3</v>
-      </c>
-      <c r="C3" s="4">
+        <f t="shared" ref="B3" si="0">A3/12</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>0.76512965913807485</v>
+      <c r="C3">
+        <f t="shared" ref="C3:C9" si="1">D3*0.0001</f>
+        <v>8.970113372800001E-3</v>
+      </c>
+      <c r="D3" s="2">
+        <v>89.701133728000002</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>24</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>7.6512965913807483E-3</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>0.79993264917340767</v>
+        <f t="shared" ref="B4:B9" si="2">A4/12</f>
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>9.4659866333000001E-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>94.659866332999997</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>36</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>7.9993264917340764E-3</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>0.84722222812211745</v>
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>9.8413871765100011E-3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>98.413871765099998</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>48</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>8.4722222812211746E-3</v>
-      </c>
-      <c r="C6" s="4">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>0.90053184539969944</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>1.0842559432980001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>108.42559432980001</v>
+      </c>
+      <c r="F6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>60</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>9.0053184539969945E-3</v>
-      </c>
-      <c r="C7" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
-        <v>0.95606556439557744</v>
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>1.1395542907710001E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>113.95542907710001</v>
+      </c>
+      <c r="F7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>84</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>9.5606556439557736E-3</v>
-      </c>
-      <c r="C8" s="4">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>1.0116682594176742</v>
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>1.210885848999E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>121.0885848999</v>
+      </c>
+      <c r="F8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>120</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>1.0116682594176743E-2</v>
-      </c>
-      <c r="C9" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>1.0661472831649033</v>
-      </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>1.0661472831649033E-2</v>
-      </c>
-      <c r="C10" s="5">
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>1.1189161304229813</v>
-      </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>1.1189161304229813E-2</v>
-      </c>
-      <c r="C11" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>1.1697595209056226</v>
-      </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>1.1697595209056227E-2</v>
-      </c>
-      <c r="C12" s="5">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="1">
-        <v>1.2186913841294837</v>
-      </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>1.2186913841294838E-2</v>
-      </c>
-      <c r="C13" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
-        <v>1.2658400685316418</v>
-      </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>1.2658400685316418E-2</v>
-      </c>
-      <c r="C14" s="5">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>1.3113708849466152</v>
-      </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>1.3113708849466152E-2</v>
-      </c>
-      <c r="C15" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>1.3554354856683479</v>
-      </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1.3554354856683479E-2</v>
-      </c>
-      <c r="C16" s="5">
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>1.398147173164731</v>
-      </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>1.3981471731647311E-2</v>
-      </c>
-      <c r="C17" s="5">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>1.439579062599309</v>
-      </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>1.4395790625993089E-2</v>
-      </c>
-      <c r="C18" s="5">
-        <v>8.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="1">
-        <v>1.4797662889469168</v>
-      </c>
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>1.4797662889469168E-2</v>
-      </c>
-      <c r="C19" s="5">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
-        <v>1.5187113555377778</v>
-      </c>
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>1.5187113555377779E-2</v>
-      </c>
-      <c r="C20" s="5">
-        <v>9.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
-        <v>1.5563891771978171</v>
-      </c>
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1.556389177197817E-2</v>
-      </c>
-      <c r="C21" s="5">
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>1.5927557618344945</v>
-      </c>
-      <c r="B22">
-        <f t="shared" si="0"/>
-        <v>1.5927557618344947E-2</v>
-      </c>
-      <c r="C22" s="5">
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>1.627752949036102</v>
-      </c>
-      <c r="B23">
-        <f t="shared" si="0"/>
-        <v>1.6277529490361022E-2</v>
-      </c>
-      <c r="C23" s="5">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>1.6613236262807265</v>
-      </c>
-      <c r="B24">
-        <f t="shared" si="0"/>
-        <v>1.6613236262807266E-2</v>
-      </c>
-      <c r="C24" s="5">
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="1">
-        <v>1.6934152853734599</v>
-      </c>
-      <c r="B25">
-        <f t="shared" si="0"/>
-        <v>1.6934152853734598E-2</v>
-      </c>
-      <c r="C25" s="5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="1">
-        <v>1.7239792810951982</v>
-      </c>
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>1.7239792810951983E-2</v>
-      </c>
-      <c r="C26" s="5">
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="1">
-        <v>1.7529745565451949</v>
-      </c>
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>1.7529745565451949E-2</v>
-      </c>
-      <c r="C27" s="5">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>1.7803741636598349</v>
-      </c>
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>1.7803741636598348E-2</v>
-      </c>
-      <c r="C28" s="5">
-        <v>13.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>1.8061642647584863</v>
-      </c>
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>1.8061642647584863E-2</v>
-      </c>
-      <c r="C29" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="1">
-        <v>1.8303428713728076</v>
-      </c>
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>1.8303428713728077E-2</v>
-      </c>
-      <c r="C30" s="5">
-        <v>14.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>1.8529196109680839</v>
-      </c>
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>1.8529196109680839E-2</v>
-      </c>
-      <c r="C31" s="5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>1.8739141735445437</v>
-      </c>
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>1.8739141735445438E-2</v>
-      </c>
-      <c r="C32" s="5">
-        <v>15.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="1">
-        <v>1.8933547400396706</v>
-      </c>
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>1.8933547400396707E-2</v>
-      </c>
-      <c r="C33" s="5">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="1">
-        <v>1.9112767162113791</v>
-      </c>
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>1.911276716211379E-2</v>
-      </c>
-      <c r="C34" s="5">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>1.9277217875947581</v>
-      </c>
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>1.9277217875947581E-2</v>
-      </c>
-      <c r="C35" s="5">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="1">
-        <v>1.9427370915825841</v>
-      </c>
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>1.9427370915825842E-2</v>
-      </c>
-      <c r="C36" s="5">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="1">
-        <v>1.9563739207142961</v>
-      </c>
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>1.9563739207142959E-2</v>
-      </c>
-      <c r="C37" s="5">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>1.968684050984419</v>
-      </c>
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>1.9686840509844192E-2</v>
-      </c>
-      <c r="C38" s="5">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>1.9797178349578859</v>
-      </c>
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>1.9797178349578858E-2</v>
-      </c>
-      <c r="C39" s="5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>1.9895243051730016</v>
-      </c>
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>1.9895243051730016E-2</v>
-      </c>
-      <c r="C40" s="5">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>1.9981513391447703</v>
-      </c>
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>1.9981513391447703E-2</v>
-      </c>
-      <c r="C41" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>2.0056457476480816</v>
-      </c>
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>2.0056457476480816E-2</v>
-      </c>
-      <c r="C42" s="5">
-        <v>20.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>2.0120519901173344</v>
-      </c>
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>2.0120519901173344E-2</v>
-      </c>
-      <c r="C43" s="5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>2.0174101476459754</v>
-      </c>
-      <c r="B44">
-        <f t="shared" si="0"/>
-        <v>2.0174101476459753E-2</v>
-      </c>
-      <c r="C44" s="5">
-        <v>21.5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
-        <v>2.0217573495520753</v>
-      </c>
-      <c r="B45">
-        <f t="shared" si="0"/>
-        <v>2.0217573495520752E-2</v>
-      </c>
-      <c r="C45" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
-        <v>2.0251289801612935</v>
-      </c>
-      <c r="B46">
-        <f t="shared" si="0"/>
-        <v>2.0251289801612934E-2</v>
-      </c>
-      <c r="C46" s="5">
-        <v>22.5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
-        <v>2.0275595983600017</v>
-      </c>
-      <c r="B47">
-        <f t="shared" si="0"/>
-        <v>2.0275595983600018E-2</v>
-      </c>
-      <c r="C47" s="5">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="1">
-        <v>2.0290842880828004</v>
-      </c>
-      <c r="B48">
-        <f t="shared" si="0"/>
-        <v>2.0290842880828004E-2</v>
-      </c>
-      <c r="C48" s="5">
-        <v>23.5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>2.0297388467590118</v>
-      </c>
-      <c r="B49">
-        <f t="shared" si="0"/>
-        <v>2.0297388467590119E-2</v>
-      </c>
-      <c r="C49" s="5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
-        <v>2.0295597395088429</v>
-      </c>
-      <c r="B50">
-        <f t="shared" si="0"/>
-        <v>2.0295597395088429E-2</v>
-      </c>
-      <c r="C50" s="5">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>2.0285847752476664</v>
-      </c>
-      <c r="B51">
-        <f t="shared" si="0"/>
-        <v>2.0285847752476664E-2</v>
-      </c>
-      <c r="C51" s="5">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>2.0268543512710573</v>
-      </c>
-      <c r="B52">
-        <f t="shared" si="0"/>
-        <v>2.0268543512710572E-2</v>
-      </c>
-      <c r="C52" s="5">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>2.0244116538022507</v>
-      </c>
-      <c r="B53">
-        <f t="shared" si="0"/>
-        <v>2.0244116538022508E-2</v>
-      </c>
-      <c r="C53" s="5">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>2.0213029785141878</v>
-      </c>
-      <c r="B54">
-        <f t="shared" si="0"/>
-        <v>2.0213029785141879E-2</v>
-      </c>
-      <c r="C54" s="5">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>2.0175774747600119</v>
-      </c>
-      <c r="B55">
-        <f t="shared" si="0"/>
-        <v>2.0175774747600118E-2</v>
-      </c>
-      <c r="C55" s="5">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>2.0132863100478877</v>
-      </c>
-      <c r="B56">
-        <f t="shared" si="0"/>
-        <v>2.0132863100478876E-2</v>
-      </c>
-      <c r="C56" s="5">
-        <v>27.5</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>2.0084822799182072</v>
-      </c>
-      <c r="B57">
-        <f t="shared" si="0"/>
-        <v>2.008482279918207E-2</v>
-      </c>
-      <c r="C57" s="5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
-        <v>2.0032196414153747</v>
-      </c>
-      <c r="B58">
-        <f t="shared" si="0"/>
-        <v>2.0032196414153748E-2</v>
-      </c>
-      <c r="C58" s="5">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>1.9975534145387082</v>
-      </c>
-      <c r="B59">
-        <f t="shared" si="0"/>
-        <v>1.997553414538708E-2</v>
-      </c>
-      <c r="C59" s="5">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>1.99153800135746</v>
-      </c>
-      <c r="B60">
-        <f t="shared" si="0"/>
-        <v>1.99153800135746E-2</v>
-      </c>
-      <c r="C60" s="5">
-        <v>29.5</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>1.9852261944736576</v>
-      </c>
-      <c r="B61">
-        <f t="shared" si="0"/>
-        <v>1.9852261944736577E-2</v>
-      </c>
-      <c r="C61" s="5">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>1.9786690136576981</v>
-      </c>
-      <c r="B62">
-        <f t="shared" si="0"/>
-        <v>1.9786690136576982E-2</v>
-      </c>
-      <c r="C62" s="5">
-        <v>30.5</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>1.9719157633862983</v>
-      </c>
-      <c r="B63">
-        <f t="shared" si="0"/>
-        <v>1.9719157633862984E-2</v>
-      </c>
-      <c r="C63" s="5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>1.9650138865784179</v>
-      </c>
-      <c r="B64">
-        <f t="shared" si="0"/>
-        <v>1.9650138865784178E-2</v>
-      </c>
-      <c r="C64" s="5">
-        <v>31.5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>1.9580086340046001</v>
-      </c>
-      <c r="B65">
-        <f t="shared" si="0"/>
-        <v>1.9580086340046002E-2</v>
-      </c>
-      <c r="C65" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <v>1.9509425199502524</v>
-      </c>
-      <c r="B66">
-        <f t="shared" si="0"/>
-        <v>1.9509425199502523E-2</v>
-      </c>
-      <c r="C66" s="5">
-        <v>32.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <v>1.9438553879025715</v>
-      </c>
-      <c r="B67">
-        <f t="shared" ref="B67:B81" si="1">A67/100</f>
-        <v>1.9438553879025714E-2</v>
-      </c>
-      <c r="C67" s="5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <v>1.9367846094794383</v>
-      </c>
-      <c r="B68">
-        <f t="shared" si="1"/>
-        <v>1.9367846094794382E-2</v>
-      </c>
-      <c r="C68" s="5">
-        <v>33.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <v>1.9297652641804675</v>
-      </c>
-      <c r="B69">
-        <f t="shared" si="1"/>
-        <v>1.9297652641804674E-2</v>
-      </c>
-      <c r="C69" s="5">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
-        <v>1.9228301085760584</v>
-      </c>
-      <c r="B70">
-        <f t="shared" si="1"/>
-        <v>1.9228301085760582E-2</v>
-      </c>
-      <c r="C70" s="5">
-        <v>34.5</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
-        <v>1.9160090894949462</v>
-      </c>
-      <c r="B71">
-        <f t="shared" si="1"/>
-        <v>1.9160090894949463E-2</v>
-      </c>
-      <c r="C71" s="5">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="1">
-        <v>1.9093293059487111</v>
-      </c>
-      <c r="B72">
-        <f t="shared" si="1"/>
-        <v>1.909329305948711E-2</v>
-      </c>
-      <c r="C72" s="5">
-        <v>35.5</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="1">
-        <v>1.9028152029879071</v>
-      </c>
-      <c r="B73">
-        <f t="shared" si="1"/>
-        <v>1.9028152029879071E-2</v>
-      </c>
-      <c r="C73" s="5">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="1">
-        <v>1.8964887534802075</v>
-      </c>
-      <c r="B74">
-        <f t="shared" si="1"/>
-        <v>1.8964887534802074E-2</v>
-      </c>
-      <c r="C74" s="5">
-        <v>36.5</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="1">
-        <v>1.890369625149797</v>
-      </c>
-      <c r="B75">
-        <f t="shared" si="1"/>
-        <v>1.8903696251497969E-2</v>
-      </c>
-      <c r="C75" s="5">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="1">
-        <v>1.8844753323633274</v>
-      </c>
-      <c r="B76">
-        <f t="shared" si="1"/>
-        <v>1.8844753323633275E-2</v>
-      </c>
-      <c r="C76" s="5">
-        <v>37.5</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="1">
-        <v>1.8788213219358558</v>
-      </c>
-      <c r="B77">
-        <f t="shared" si="1"/>
-        <v>1.8788213219358557E-2</v>
-      </c>
-      <c r="C77" s="5">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="1">
-        <v>1.8734210007897918</v>
-      </c>
-      <c r="B78">
-        <f t="shared" si="1"/>
-        <v>1.873421000789792E-2</v>
-      </c>
-      <c r="C78" s="5">
-        <v>38.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="1">
-        <v>1.8682858444945127</v>
-      </c>
-      <c r="B79">
-        <f t="shared" si="1"/>
-        <v>1.8682858444945126E-2</v>
-      </c>
-      <c r="C79" s="5">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="1">
-        <v>1.8634254502936896</v>
-      </c>
-      <c r="B80">
-        <f t="shared" si="1"/>
-        <v>1.8634254502936896E-2</v>
-      </c>
-      <c r="C80" s="5">
-        <v>39.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="1">
-        <v>1.8588474188546644</v>
-      </c>
-      <c r="B81">
-        <f t="shared" si="1"/>
-        <v>1.8588474188546644E-2</v>
-      </c>
-      <c r="C81" s="5">
-        <v>40</v>
-      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>1.2994847106930002E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>129.94847106930001</v>
+      </c>
+      <c r="F9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2497,172 +1665,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF84E3C-6123-564C-ACEF-26D67C5C8B64}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="0" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2">
-        <f>A2/12</f>
-        <v>0.5</v>
-      </c>
-      <c r="C2">
-        <f>D2*0.0001</f>
-        <v>8.1129268646200001E-3</v>
-      </c>
-      <c r="D2" s="2">
-        <v>81.129268646200003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B9" si="0">A3/12</f>
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C9" si="1">D3*0.0001</f>
-        <v>8.970113372800001E-3</v>
-      </c>
-      <c r="D3" s="2">
-        <v>89.701133728000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>24</v>
-      </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <f t="shared" si="1"/>
-        <v>9.4659866333000001E-3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>94.659866332999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>36</v>
-      </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <f t="shared" si="1"/>
-        <v>9.8413871765100011E-3</v>
-      </c>
-      <c r="D5" s="2">
-        <v>98.413871765099998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>48</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <f t="shared" si="1"/>
-        <v>1.0842559432980001E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>108.42559432980001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>60</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <f t="shared" si="1"/>
-        <v>1.1395542907710001E-2</v>
-      </c>
-      <c r="D7" s="2">
-        <v>113.95542907710001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>84</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <f t="shared" si="1"/>
-        <v>1.210885848999E-2</v>
-      </c>
-      <c r="D8" s="2">
-        <v>121.0885848999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>120</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <f t="shared" si="1"/>
-        <v>1.2994847106930002E-2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>129.94847106930001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{676432AF-0F53-454C-A2CE-3A93B5AF25D7}">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2709,11 +1716,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE280868-0661-6A4B-9B03-0147465E5A5C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Calibarte CDS params, sigmoid function for survivourship, liquidity risk step increase function, vol, and yield curve stress
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2764405r_student_gla_ac_uk/Documents/Industry Project/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kasiraj/Library/CloudStorage/OneDrive-UniversityofGlasgow/Industry Project/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{8EF8A760-6F87-3F47-B0D2-BB4510910C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB22C586-A602-C341-9088-DF4A6ADD63F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F5653F-24E5-4D41-8523-900C80DDA27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="1700" windowWidth="26700" windowHeight="16940" activeTab="1" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
+    <workbookView xWindow="3920" yWindow="1320" windowWidth="26700" windowHeight="16940" activeTab="3" xr2:uid="{DE38C1C5-30E6-D742-B48E-E8325D0BF4FB}"/>
   </bookViews>
   <sheets>
     <sheet name="interest_rate_term_structure" sheetId="1" r:id="rId1"/>
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B238863E-1E4E-CE48-8256-D2C0605750DF}">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="B2" sqref="A1:D65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1499,8 +1499,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF84E3C-6123-564C-ACEF-26D67C5C8B64}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1669,7 +1669,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1693,7 +1693,7 @@
         <v>0.52890499999999996</v>
       </c>
       <c r="B2">
-        <v>2.6499999999999999E-2</v>
+        <v>3.1990400000000002E-2</v>
       </c>
       <c r="C2">
         <v>0.13003500000000001</v>
@@ -1718,10 +1718,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE280868-0661-6A4B-9B03-0147465E5A5C}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1751,16 +1751,16 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.35420099999999999</v>
+        <v>0.35590523000000002</v>
       </c>
       <c r="B2">
-        <v>1.21853E-3</v>
+        <v>1.49927E-3</v>
       </c>
       <c r="C2">
-        <v>2.38186E-3</v>
+        <v>2.3764799999999998E-3</v>
       </c>
       <c r="D2">
-        <v>1.81E-3</v>
+        <v>1.97182E-3</v>
       </c>
       <c r="E2">
         <v>0.4</v>
@@ -1769,7 +1769,148 @@
         <v>4</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>6.0976130000000003E-2</v>
+      </c>
+      <c r="B3">
+        <v>2.8177200000000001E-3</v>
+      </c>
+      <c r="C3">
+        <v>0.37078147</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>9.7805409999999995E-2</v>
+      </c>
+      <c r="B4">
+        <v>5.7516999999999996E-4</v>
+      </c>
+      <c r="C4">
+        <v>0.12454273</v>
+      </c>
+      <c r="D4">
+        <v>2.9165900000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>0.35420099999999999</v>
+      </c>
+      <c r="B5">
+        <v>1.21853E-3</v>
+      </c>
+      <c r="C5">
+        <v>2.38186E-3</v>
+      </c>
+      <c r="D5">
+        <v>1.81E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>0.37079495000000001</v>
+      </c>
+      <c r="B6">
+        <v>3.8134200000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>2.50118E-3</v>
+      </c>
+      <c r="D6">
+        <v>2.1209900000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>0.37072224999999998</v>
+      </c>
+      <c r="B7">
+        <v>3.09399E-3</v>
+      </c>
+      <c r="C7">
+        <v>2.5071500000000001E-3</v>
+      </c>
+      <c r="D7">
+        <v>3.6718499999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>0.36948254000000003</v>
+      </c>
+      <c r="B8">
+        <v>3.8684E-4</v>
+      </c>
+      <c r="C8">
+        <v>2.4764700000000001E-3</v>
+      </c>
+      <c r="D8">
+        <v>9.8715000000000001E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>0.63004337399999999</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.2447731499999999E-4</v>
+      </c>
+      <c r="C9" s="3">
+        <v>4.1979461500000004E-3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.51173503E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0.42458847999999999</v>
+      </c>
+      <c r="B10">
+        <v>4.0863699999999998E-3</v>
+      </c>
+      <c r="C10">
+        <v>2.8134100000000001E-3</v>
+      </c>
+      <c r="D10">
+        <v>1.1898099999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>0.38846364</v>
+      </c>
+      <c r="B11">
+        <v>1.10464E-3</v>
+      </c>
+      <c r="C11">
+        <v>2.59129E-3</v>
+      </c>
+      <c r="D11">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>0.35590523000000002</v>
+      </c>
+      <c r="B12">
+        <v>1.49927E-3</v>
+      </c>
+      <c r="C12">
+        <v>2.3764799999999998E-3</v>
+      </c>
+      <c r="D12">
+        <v>1.97182E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>